<commit_message>
sound tiresqueaking implemented in program
</commit_message>
<xml_diff>
--- a/Daan logboek.xlsx
+++ b/Daan logboek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7a575cd3af734844/Bureaublad/wk 12/Challenge_Week-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{E5B1702C-8CBE-4EDB-9542-D877C8874A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{45DF977E-9477-4697-B68F-95D343385433}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{E5B1702C-8CBE-4EDB-9542-D877C8874A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E686F878-0532-4BDE-B0E3-16CB5AA5FB84}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>datum</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>de auto veranderd nu altijd of het scherm is zwart</t>
+  </si>
+  <si>
+    <t>sound for tire squeaking</t>
   </si>
 </sst>
 </file>
@@ -457,7 +460,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,6 +611,12 @@
       <c r="A10" s="1">
         <v>45261</v>
       </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>